<commit_message>
project2_gg --- get_hotels returns 3 hotels instead of 1 now, also did debugging
</commit_message>
<xml_diff>
--- a/customerqueue/srtr1.xlsx
+++ b/customerqueue/srtr1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\customerqueue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5A8671-A4DB-490F-ADDB-F46010252DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CAD7B0-59F2-4515-B15D-0E26E27D5E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="2340" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>$100 to $299</t>
+  </si>
+  <si>
+    <t>1 Room</t>
   </si>
 </sst>
 </file>
@@ -75,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -557,7 +560,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,7 +943,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,8 +999,8 @@
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="G2" t="s">
+        <v>16</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -1025,8 +1028,8 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3">
-        <v>1</v>
+      <c r="G3" t="s">
+        <v>16</v>
       </c>
       <c r="H3">
         <v>2</v>

</xml_diff>